<commit_message>
Wood & new ArmyArea
Primi modellini poliglonali di environment (bosco e roccia)
Passive skill system, tra cui implementazione del bosco come oggetto che riduce precisione di attacchi ricevuti
Revisione delle army areas per gestire il movimento che si raddoppia passando nel bosco
Piccole modifiche a camera e camera apposita per areas
</commit_message>
<xml_diff>
--- a/GameDesign/Eserciti.xlsx
+++ b/GameDesign/Eserciti.xlsx
@@ -353,32 +353,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Explosive Shell </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(melee attack, fire element, Att 6; self damage: fire element, Att 3, precision 0.2): </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">the shells are filled with gunpowder and can create dangerous explosions while attacking. This is a risky move, the unit receive in fact a damage due to the runaway explosions. </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Bubble cannon </t>
     </r>
     <r>
@@ -962,6 +936,32 @@
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Explosive Shell </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(melee attack, fire element, Att + 1.5; self damage: fire element, Att 3, precision 0.2): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">the shells are filled with gunpowder and can create dangerous explosions while attacking. This is a risky move, the unit receive in fact a damage due to the runaway explosions. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1426,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,7 +1603,7 @@
         <v>4</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1680,7 +1680,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1688,10 +1688,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>29</v>
@@ -1699,12 +1699,12 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H25" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H26" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1754,7 +1754,7 @@
         <v>8</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1771,7 +1771,7 @@
         <v>18</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1820,7 +1820,7 @@
         <v>34</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1837,7 +1837,7 @@
         <v>7</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1886,17 +1886,17 @@
         <v>1</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H42" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H43" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1939,7 +1939,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2069,7 +2069,7 @@
         <v>4</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2135,7 +2135,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2202,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2210,7 +2210,7 @@
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="H23" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="H25" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2236,7 +2236,7 @@
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="H26" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2245,7 +2245,7 @@
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="H27" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2268,13 +2268,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="H35" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2288,12 +2288,12 @@
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="H36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="9">
         <v>4</v>

</xml_diff>